<commit_message>
poner bonito el excel
</commit_message>
<xml_diff>
--- a/ITER1/ARTEFACTOS/ARTEFACTO 7.xlsx
+++ b/ITER1/ARTEFACTOS/ARTEFACTO 7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidaddealcala-my.sharepoint.com/personal/miguel_losada_edu_uah_es/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{313B58E7-3250-4B62-8FEA-35152025FD98}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8421EBB-73A1-46D0-90EA-B740FAEA9DED}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7632" activeTab="1" xr2:uid="{D68F269D-CCB5-4930-8DCD-09FEBB86FD79}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" activeTab="1" xr2:uid="{D68F269D-CCB5-4930-8DCD-09FEBB86FD79}"/>
   </bookViews>
   <sheets>
     <sheet name="ARTEFACTO7.1" sheetId="2" r:id="rId1"/>
@@ -312,7 +312,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -534,11 +534,41 @@
         <color auto="1"/>
       </diagonal>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="thick">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -616,6 +646,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -935,16 +971,16 @@
   <dimension ref="A1:BV14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="2"/>
-    <col min="2" max="16384" width="11.44140625" style="3"/>
+    <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="2" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" s="5" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:74" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1166,7 +1202,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>73</v>
       </c>
@@ -1244,7 +1280,7 @@
       <c r="BU2" s="16"/>
       <c r="BV2" s="17"/>
     </row>
-    <row r="3" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>74</v>
       </c>
@@ -1322,7 +1358,7 @@
       <c r="BU3" s="19"/>
       <c r="BV3" s="20"/>
     </row>
-    <row r="4" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>75</v>
       </c>
@@ -1400,7 +1436,7 @@
       <c r="BU4" s="19"/>
       <c r="BV4" s="20"/>
     </row>
-    <row r="5" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>76</v>
       </c>
@@ -1478,7 +1514,7 @@
       <c r="BU5" s="19"/>
       <c r="BV5" s="20"/>
     </row>
-    <row r="6" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>77</v>
       </c>
@@ -1556,7 +1592,7 @@
       <c r="BU6" s="19"/>
       <c r="BV6" s="20"/>
     </row>
-    <row r="7" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>78</v>
       </c>
@@ -1634,7 +1670,7 @@
       <c r="BU7" s="19"/>
       <c r="BV7" s="20"/>
     </row>
-    <row r="8" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>79</v>
       </c>
@@ -1712,7 +1748,7 @@
       <c r="BU8" s="19"/>
       <c r="BV8" s="20"/>
     </row>
-    <row r="9" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>80</v>
       </c>
@@ -1790,7 +1826,7 @@
       <c r="BU9" s="19"/>
       <c r="BV9" s="20"/>
     </row>
-    <row r="10" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>81</v>
       </c>
@@ -1868,7 +1904,7 @@
       <c r="BU10" s="19"/>
       <c r="BV10" s="20"/>
     </row>
-    <row r="11" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>82</v>
       </c>
@@ -1946,7 +1982,7 @@
       <c r="BU11" s="19"/>
       <c r="BV11" s="20"/>
     </row>
-    <row r="12" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>83</v>
       </c>
@@ -2024,7 +2060,7 @@
       <c r="BU12" s="19"/>
       <c r="BV12" s="20"/>
     </row>
-    <row r="13" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>84</v>
       </c>
@@ -2102,7 +2138,7 @@
       <c r="BU13" s="22"/>
       <c r="BV13" s="23"/>
     </row>
-    <row r="14" spans="1:74" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:74" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2112,17 +2148,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F115FB-91EA-4D3D-AC52-FEB512D0E00D}">
   <dimension ref="A1:BV106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z56" sqref="Z56"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BJ103" sqref="BJ103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="5"/>
-    <col min="2" max="16384" width="11.44140625" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="5"/>
+    <col min="2" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" s="5" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:74" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -2344,7 +2380,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2422,7 +2458,7 @@
       <c r="BU2" s="8"/>
       <c r="BV2" s="9"/>
     </row>
-    <row r="3" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2500,7 +2536,7 @@
       <c r="BU3" s="11"/>
       <c r="BV3" s="12"/>
     </row>
-    <row r="4" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2578,7 +2614,7 @@
       <c r="BU4" s="11"/>
       <c r="BV4" s="12"/>
     </row>
-    <row r="5" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2656,7 +2692,7 @@
       <c r="BU5" s="11"/>
       <c r="BV5" s="24"/>
     </row>
-    <row r="6" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2734,7 +2770,7 @@
       <c r="BU6" s="11"/>
       <c r="BV6" s="24"/>
     </row>
-    <row r="7" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2752,8 +2788,8 @@
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
@@ -2812,7 +2848,7 @@
       <c r="BU7" s="11"/>
       <c r="BV7" s="12"/>
     </row>
-    <row r="8" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2830,8 +2866,8 @@
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
       <c r="T8" s="11"/>
@@ -2890,7 +2926,7 @@
       <c r="BU8" s="11"/>
       <c r="BV8" s="12"/>
     </row>
-    <row r="9" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2908,8 +2944,8 @@
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
       <c r="T9" s="11"/>
@@ -2968,7 +3004,7 @@
       <c r="BU9" s="11"/>
       <c r="BV9" s="12"/>
     </row>
-    <row r="10" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2986,8 +3022,8 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
@@ -3046,7 +3082,7 @@
       <c r="BU10" s="11"/>
       <c r="BV10" s="12"/>
     </row>
-    <row r="11" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3064,8 +3100,8 @@
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
       <c r="T11" s="11"/>
@@ -3124,7 +3160,7 @@
       <c r="BU11" s="11"/>
       <c r="BV11" s="12"/>
     </row>
-    <row r="12" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3142,8 +3178,8 @@
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
       <c r="T12" s="11"/>
@@ -3202,7 +3238,7 @@
       <c r="BU12" s="11"/>
       <c r="BV12" s="12"/>
     </row>
-    <row r="13" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3220,8 +3256,8 @@
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
       <c r="T13" s="11"/>
@@ -3280,7 +3316,7 @@
       <c r="BU13" s="11"/>
       <c r="BV13" s="12"/>
     </row>
-    <row r="14" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3298,8 +3334,8 @@
       <c r="M14" s="11"/>
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
       <c r="T14" s="11"/>
@@ -3358,7 +3394,7 @@
       <c r="BU14" s="11"/>
       <c r="BV14" s="12"/>
     </row>
-    <row r="15" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -3374,7 +3410,7 @@
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
-      <c r="N15" s="24"/>
+      <c r="N15" s="25"/>
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
@@ -3436,7 +3472,7 @@
       <c r="BU15" s="11"/>
       <c r="BV15" s="12"/>
     </row>
-    <row r="16" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -3452,7 +3488,7 @@
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
-      <c r="N16" s="24"/>
+      <c r="N16" s="25"/>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
@@ -3514,7 +3550,7 @@
       <c r="BU16" s="11"/>
       <c r="BV16" s="12"/>
     </row>
-    <row r="17" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -3530,7 +3566,7 @@
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
-      <c r="N17" s="24"/>
+      <c r="N17" s="25"/>
       <c r="O17" s="11"/>
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
@@ -3592,7 +3628,7 @@
       <c r="BU17" s="11"/>
       <c r="BV17" s="12"/>
     </row>
-    <row r="18" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -3608,7 +3644,7 @@
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
-      <c r="N18" s="24"/>
+      <c r="N18" s="25"/>
       <c r="O18" s="11"/>
       <c r="P18" s="11"/>
       <c r="Q18" s="11"/>
@@ -3670,7 +3706,7 @@
       <c r="BU18" s="11"/>
       <c r="BV18" s="12"/>
     </row>
-    <row r="19" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -3683,17 +3719,17 @@
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
       <c r="O19" s="11"/>
       <c r="P19" s="11"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
-      <c r="T19" s="24"/>
-      <c r="U19" s="24"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
+      <c r="T19" s="25"/>
+      <c r="U19" s="25"/>
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
       <c r="X19" s="11"/>
@@ -3708,8 +3744,8 @@
       <c r="AG19" s="11"/>
       <c r="AH19" s="11"/>
       <c r="AI19" s="11"/>
-      <c r="AJ19" s="24"/>
-      <c r="AK19" s="24"/>
+      <c r="AJ19" s="25"/>
+      <c r="AK19" s="25"/>
       <c r="AL19" s="11"/>
       <c r="AM19" s="11"/>
       <c r="AN19" s="11"/>
@@ -3748,7 +3784,7 @@
       <c r="BU19" s="11"/>
       <c r="BV19" s="12"/>
     </row>
-    <row r="20" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -3761,17 +3797,17 @@
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
       <c r="O20" s="11"/>
       <c r="P20" s="11"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="25"/>
+      <c r="U20" s="25"/>
       <c r="V20" s="11"/>
       <c r="W20" s="11"/>
       <c r="X20" s="11"/>
@@ -3786,8 +3822,8 @@
       <c r="AG20" s="11"/>
       <c r="AH20" s="11"/>
       <c r="AI20" s="11"/>
-      <c r="AJ20" s="24"/>
-      <c r="AK20" s="24"/>
+      <c r="AJ20" s="25"/>
+      <c r="AK20" s="25"/>
       <c r="AL20" s="11"/>
       <c r="AM20" s="11"/>
       <c r="AN20" s="11"/>
@@ -3826,7 +3862,7 @@
       <c r="BU20" s="11"/>
       <c r="BV20" s="12"/>
     </row>
-    <row r="21" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -3839,17 +3875,17 @@
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
       <c r="O21" s="11"/>
       <c r="P21" s="11"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
+      <c r="S21" s="25"/>
+      <c r="T21" s="25"/>
+      <c r="U21" s="25"/>
       <c r="V21" s="11"/>
       <c r="W21" s="11"/>
       <c r="X21" s="11"/>
@@ -3864,8 +3900,8 @@
       <c r="AG21" s="11"/>
       <c r="AH21" s="11"/>
       <c r="AI21" s="11"/>
-      <c r="AJ21" s="24"/>
-      <c r="AK21" s="24"/>
+      <c r="AJ21" s="25"/>
+      <c r="AK21" s="25"/>
       <c r="AL21" s="11"/>
       <c r="AM21" s="11"/>
       <c r="AN21" s="11"/>
@@ -3904,7 +3940,7 @@
       <c r="BU21" s="11"/>
       <c r="BV21" s="12"/>
     </row>
-    <row r="22" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -3916,7 +3952,7 @@
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
-      <c r="J22" s="24"/>
+      <c r="J22" s="25"/>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
       <c r="M22" s="11"/>
@@ -3982,7 +4018,7 @@
       <c r="BU22" s="11"/>
       <c r="BV22" s="12"/>
     </row>
-    <row r="23" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -3994,7 +4030,7 @@
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
-      <c r="J23" s="24"/>
+      <c r="J23" s="25"/>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
@@ -4060,7 +4096,7 @@
       <c r="BU23" s="11"/>
       <c r="BV23" s="12"/>
     </row>
-    <row r="24" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -4072,7 +4108,7 @@
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
-      <c r="J24" s="24"/>
+      <c r="J24" s="25"/>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
       <c r="M24" s="11"/>
@@ -4138,7 +4174,7 @@
       <c r="BU24" s="11"/>
       <c r="BV24" s="12"/>
     </row>
-    <row r="25" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -4150,7 +4186,7 @@
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
-      <c r="J25" s="24"/>
+      <c r="J25" s="25"/>
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
       <c r="M25" s="11"/>
@@ -4216,7 +4252,7 @@
       <c r="BU25" s="11"/>
       <c r="BV25" s="12"/>
     </row>
-    <row r="26" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -4228,7 +4264,7 @@
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
-      <c r="J26" s="24"/>
+      <c r="J26" s="25"/>
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
@@ -4294,7 +4330,7 @@
       <c r="BU26" s="11"/>
       <c r="BV26" s="12"/>
     </row>
-    <row r="27" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -4306,7 +4342,7 @@
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
-      <c r="J27" s="24"/>
+      <c r="J27" s="25"/>
       <c r="K27" s="11"/>
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
@@ -4372,7 +4408,7 @@
       <c r="BU27" s="11"/>
       <c r="BV27" s="12"/>
     </row>
-    <row r="28" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -4384,7 +4420,7 @@
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
-      <c r="J28" s="24"/>
+      <c r="J28" s="25"/>
       <c r="K28" s="11"/>
       <c r="L28" s="11"/>
       <c r="M28" s="11"/>
@@ -4450,7 +4486,7 @@
       <c r="BU28" s="11"/>
       <c r="BV28" s="12"/>
     </row>
-    <row r="29" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -4462,7 +4498,7 @@
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
-      <c r="J29" s="24"/>
+      <c r="J29" s="25"/>
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
@@ -4528,7 +4564,7 @@
       <c r="BU29" s="11"/>
       <c r="BV29" s="12"/>
     </row>
-    <row r="30" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -4540,7 +4576,7 @@
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
-      <c r="J30" s="24"/>
+      <c r="J30" s="25"/>
       <c r="K30" s="11"/>
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
@@ -4606,7 +4642,7 @@
       <c r="BU30" s="11"/>
       <c r="BV30" s="12"/>
     </row>
-    <row r="31" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -4618,7 +4654,7 @@
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="25"/>
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
       <c r="M31" s="11"/>
@@ -4684,7 +4720,7 @@
       <c r="BU31" s="11"/>
       <c r="BV31" s="12"/>
     </row>
-    <row r="32" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -4712,7 +4748,7 @@
       <c r="W32" s="11"/>
       <c r="X32" s="11"/>
       <c r="Y32" s="11"/>
-      <c r="Z32" s="24"/>
+      <c r="Z32" s="25"/>
       <c r="AA32" s="11"/>
       <c r="AB32" s="11"/>
       <c r="AC32" s="11"/>
@@ -4762,7 +4798,7 @@
       <c r="BU32" s="11"/>
       <c r="BV32" s="12"/>
     </row>
-    <row r="33" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -4790,7 +4826,7 @@
       <c r="W33" s="11"/>
       <c r="X33" s="11"/>
       <c r="Y33" s="11"/>
-      <c r="Z33" s="24"/>
+      <c r="Z33" s="25"/>
       <c r="AA33" s="11"/>
       <c r="AB33" s="11"/>
       <c r="AC33" s="11"/>
@@ -4840,7 +4876,7 @@
       <c r="BU33" s="11"/>
       <c r="BV33" s="12"/>
     </row>
-    <row r="34" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -4868,7 +4904,7 @@
       <c r="W34" s="11"/>
       <c r="X34" s="11"/>
       <c r="Y34" s="11"/>
-      <c r="Z34" s="24"/>
+      <c r="Z34" s="25"/>
       <c r="AA34" s="11"/>
       <c r="AB34" s="11"/>
       <c r="AC34" s="11"/>
@@ -4918,7 +4954,7 @@
       <c r="BU34" s="11"/>
       <c r="BV34" s="12"/>
     </row>
-    <row r="35" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -4946,7 +4982,7 @@
       <c r="W35" s="11"/>
       <c r="X35" s="11"/>
       <c r="Y35" s="11"/>
-      <c r="Z35" s="24"/>
+      <c r="Z35" s="25"/>
       <c r="AA35" s="11"/>
       <c r="AB35" s="11"/>
       <c r="AC35" s="11"/>
@@ -4996,7 +5032,7 @@
       <c r="BU35" s="11"/>
       <c r="BV35" s="12"/>
     </row>
-    <row r="36" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -5024,7 +5060,7 @@
       <c r="W36" s="11"/>
       <c r="X36" s="11"/>
       <c r="Y36" s="11"/>
-      <c r="Z36" s="24"/>
+      <c r="Z36" s="25"/>
       <c r="AA36" s="11"/>
       <c r="AB36" s="11"/>
       <c r="AC36" s="11"/>
@@ -5074,7 +5110,7 @@
       <c r="BU36" s="11"/>
       <c r="BV36" s="12"/>
     </row>
-    <row r="37" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -5082,10 +5118,10 @@
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
       <c r="L37" s="11"/>
@@ -5152,7 +5188,7 @@
       <c r="BU37" s="11"/>
       <c r="BV37" s="12"/>
     </row>
-    <row r="38" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -5161,9 +5197,9 @@
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
       <c r="J38" s="11"/>
       <c r="K38" s="11"/>
       <c r="L38" s="11"/>
@@ -5230,7 +5266,7 @@
       <c r="BU38" s="11"/>
       <c r="BV38" s="12"/>
     </row>
-    <row r="39" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -5239,9 +5275,9 @@
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
       <c r="J39" s="11"/>
       <c r="K39" s="11"/>
       <c r="L39" s="11"/>
@@ -5308,7 +5344,7 @@
       <c r="BU39" s="11"/>
       <c r="BV39" s="12"/>
     </row>
-    <row r="40" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -5317,9 +5353,9 @@
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
       <c r="J40" s="11"/>
       <c r="K40" s="11"/>
       <c r="L40" s="11"/>
@@ -5386,7 +5422,7 @@
       <c r="BU40" s="11"/>
       <c r="BV40" s="12"/>
     </row>
-    <row r="41" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -5395,7 +5431,7 @@
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
-      <c r="G41" s="24"/>
+      <c r="G41" s="25"/>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="11"/>
@@ -5464,7 +5500,7 @@
       <c r="BU41" s="11"/>
       <c r="BV41" s="12"/>
     </row>
-    <row r="42" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -5473,8 +5509,8 @@
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
       <c r="I42" s="11"/>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
@@ -5542,7 +5578,7 @@
       <c r="BU42" s="11"/>
       <c r="BV42" s="12"/>
     </row>
-    <row r="43" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -5551,8 +5587,8 @@
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
       <c r="I43" s="11"/>
       <c r="J43" s="11"/>
       <c r="K43" s="11"/>
@@ -5620,7 +5656,7 @@
       <c r="BU43" s="11"/>
       <c r="BV43" s="12"/>
     </row>
-    <row r="44" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -5632,7 +5668,7 @@
       <c r="G44" s="11"/>
       <c r="H44"/>
       <c r="I44" s="11"/>
-      <c r="J44" s="24"/>
+      <c r="J44" s="25"/>
       <c r="K44" s="11"/>
       <c r="L44" s="11"/>
       <c r="M44" s="11"/>
@@ -5698,7 +5734,7 @@
       <c r="BU44" s="11"/>
       <c r="BV44" s="12"/>
     </row>
-    <row r="45" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -5711,8 +5747,8 @@
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="24"/>
+      <c r="K45" s="25"/>
+      <c r="L45" s="25"/>
       <c r="M45" s="11"/>
       <c r="N45" s="11"/>
       <c r="O45" s="11"/>
@@ -5730,12 +5766,12 @@
       <c r="AA45" s="11"/>
       <c r="AB45" s="11"/>
       <c r="AC45" s="11"/>
-      <c r="AD45" s="24"/>
-      <c r="AE45" s="24"/>
+      <c r="AD45" s="25"/>
+      <c r="AE45" s="25"/>
       <c r="AF45" s="11"/>
       <c r="AG45" s="11"/>
-      <c r="AH45" s="24"/>
-      <c r="AI45" s="24"/>
+      <c r="AH45" s="25"/>
+      <c r="AI45" s="25"/>
       <c r="AJ45" s="11"/>
       <c r="AK45" s="11"/>
       <c r="AL45" s="11"/>
@@ -5776,7 +5812,7 @@
       <c r="BU45" s="11"/>
       <c r="BV45" s="12"/>
     </row>
-    <row r="46" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -5789,8 +5825,8 @@
       <c r="H46" s="11"/>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
-      <c r="K46" s="24"/>
-      <c r="L46" s="24"/>
+      <c r="K46" s="25"/>
+      <c r="L46" s="25"/>
       <c r="M46" s="11"/>
       <c r="N46" s="11"/>
       <c r="O46" s="11"/>
@@ -5808,12 +5844,12 @@
       <c r="AA46" s="11"/>
       <c r="AB46" s="11"/>
       <c r="AC46" s="11"/>
-      <c r="AD46" s="24"/>
-      <c r="AE46" s="24"/>
+      <c r="AD46" s="25"/>
+      <c r="AE46" s="25"/>
       <c r="AF46" s="11"/>
       <c r="AG46" s="11"/>
-      <c r="AH46" s="24"/>
-      <c r="AI46" s="24"/>
+      <c r="AH46" s="25"/>
+      <c r="AI46" s="25"/>
       <c r="AJ46" s="11"/>
       <c r="AK46" s="11"/>
       <c r="AL46" s="11"/>
@@ -5854,7 +5890,7 @@
       <c r="BU46" s="11"/>
       <c r="BV46" s="12"/>
     </row>
-    <row r="47" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -5867,9 +5903,9 @@
       <c r="H47" s="11"/>
       <c r="I47" s="11"/>
       <c r="J47" s="11"/>
-      <c r="K47" s="24"/>
-      <c r="L47" s="24"/>
-      <c r="M47" s="24"/>
+      <c r="K47" s="25"/>
+      <c r="L47" s="25"/>
+      <c r="M47" s="25"/>
       <c r="N47" s="11"/>
       <c r="O47" s="11"/>
       <c r="P47" s="11"/>
@@ -5932,7 +5968,7 @@
       <c r="BU47" s="11"/>
       <c r="BV47" s="12"/>
     </row>
-    <row r="48" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -5945,10 +5981,10 @@
       <c r="H48" s="11"/>
       <c r="I48" s="11"/>
       <c r="J48" s="11"/>
-      <c r="K48" s="24"/>
-      <c r="L48" s="24"/>
+      <c r="K48" s="25"/>
+      <c r="L48" s="25"/>
       <c r="M48" s="11"/>
-      <c r="N48" s="24"/>
+      <c r="N48" s="25"/>
       <c r="O48" s="11"/>
       <c r="P48" s="11"/>
       <c r="Q48" s="11"/>
@@ -6010,7 +6046,7 @@
       <c r="BU48" s="11"/>
       <c r="BV48" s="12"/>
     </row>
-    <row r="49" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -6040,11 +6076,11 @@
       <c r="Y49" s="11"/>
       <c r="Z49" s="11"/>
       <c r="AA49" s="11"/>
-      <c r="AB49" s="24"/>
+      <c r="AB49" s="25"/>
       <c r="AC49"/>
       <c r="AD49" s="11"/>
       <c r="AE49" s="11"/>
-      <c r="AF49" s="24"/>
+      <c r="AF49" s="25"/>
       <c r="AG49"/>
       <c r="AH49" s="11"/>
       <c r="AI49" s="11"/>
@@ -6088,7 +6124,7 @@
       <c r="BU49" s="11"/>
       <c r="BV49" s="12"/>
     </row>
-    <row r="50" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -6119,11 +6155,11 @@
       <c r="Z50" s="11"/>
       <c r="AA50" s="11"/>
       <c r="AB50" s="11"/>
-      <c r="AC50" s="24"/>
+      <c r="AC50" s="25"/>
       <c r="AD50" s="11"/>
       <c r="AE50" s="11"/>
       <c r="AF50" s="11"/>
-      <c r="AG50" s="24"/>
+      <c r="AG50" s="25"/>
       <c r="AH50" s="11"/>
       <c r="AI50" s="11"/>
       <c r="AJ50" s="11"/>
@@ -6166,7 +6202,7 @@
       <c r="BU50" s="11"/>
       <c r="BV50" s="12"/>
     </row>
-    <row r="51" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -6179,8 +6215,8 @@
       <c r="H51" s="11"/>
       <c r="I51" s="11"/>
       <c r="J51" s="11"/>
-      <c r="K51" s="24"/>
-      <c r="L51" s="24"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="25"/>
       <c r="M51" s="11"/>
       <c r="N51" s="11"/>
       <c r="O51" s="11"/>
@@ -6196,11 +6232,11 @@
       <c r="Y51" s="11"/>
       <c r="Z51" s="11"/>
       <c r="AA51" s="11"/>
-      <c r="AB51" s="24"/>
+      <c r="AB51" s="25"/>
       <c r="AC51"/>
       <c r="AD51" s="11"/>
       <c r="AE51" s="11"/>
-      <c r="AF51" s="24"/>
+      <c r="AF51" s="25"/>
       <c r="AG51"/>
       <c r="AH51" s="11"/>
       <c r="AI51" s="11"/>
@@ -6244,7 +6280,7 @@
       <c r="BU51" s="11"/>
       <c r="BV51" s="12"/>
     </row>
-    <row r="52" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -6257,8 +6293,8 @@
       <c r="H52" s="11"/>
       <c r="I52" s="11"/>
       <c r="J52" s="11"/>
-      <c r="K52" s="24"/>
-      <c r="L52" s="24"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
       <c r="M52" s="11"/>
       <c r="N52" s="11"/>
       <c r="O52" s="11"/>
@@ -6275,11 +6311,11 @@
       <c r="Z52" s="11"/>
       <c r="AA52" s="11"/>
       <c r="AB52" s="11"/>
-      <c r="AC52" s="24"/>
+      <c r="AC52" s="25"/>
       <c r="AD52" s="11"/>
       <c r="AE52" s="11"/>
       <c r="AF52" s="11"/>
-      <c r="AG52" s="24"/>
+      <c r="AG52" s="25"/>
       <c r="AH52" s="11"/>
       <c r="AI52" s="11"/>
       <c r="AJ52" s="11"/>
@@ -6322,7 +6358,7 @@
       <c r="BU52" s="11"/>
       <c r="BV52" s="12"/>
     </row>
-    <row r="53" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -6339,7 +6375,7 @@
       <c r="L53" s="11"/>
       <c r="M53" s="11"/>
       <c r="N53" s="11"/>
-      <c r="O53" s="24"/>
+      <c r="O53" s="25"/>
       <c r="P53" s="11"/>
       <c r="Q53" s="11"/>
       <c r="R53" s="11"/>
@@ -6351,7 +6387,7 @@
       <c r="X53" s="11"/>
       <c r="Y53" s="11"/>
       <c r="Z53" s="11"/>
-      <c r="AA53" s="24"/>
+      <c r="AA53" s="25"/>
       <c r="AB53" s="11"/>
       <c r="AC53" s="11"/>
       <c r="AD53" s="11"/>
@@ -6400,7 +6436,7 @@
       <c r="BU53" s="11"/>
       <c r="BV53" s="12"/>
     </row>
-    <row r="54" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -6418,7 +6454,7 @@
       <c r="M54" s="11"/>
       <c r="N54" s="11"/>
       <c r="O54" s="11"/>
-      <c r="P54" s="24"/>
+      <c r="P54" s="25"/>
       <c r="Q54" s="11"/>
       <c r="R54" s="11"/>
       <c r="S54" s="11"/>
@@ -6428,7 +6464,7 @@
       <c r="W54" s="11"/>
       <c r="X54" s="11"/>
       <c r="Y54" s="11"/>
-      <c r="Z54" s="24"/>
+      <c r="Z54" s="25"/>
       <c r="AA54" s="11"/>
       <c r="AB54" s="11"/>
       <c r="AC54" s="11"/>
@@ -6478,7 +6514,7 @@
       <c r="BU54" s="11"/>
       <c r="BV54" s="12"/>
     </row>
-    <row r="55" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -6496,8 +6532,8 @@
       <c r="M55" s="11"/>
       <c r="N55" s="11"/>
       <c r="O55"/>
-      <c r="P55" s="24"/>
-      <c r="Q55" s="24"/>
+      <c r="P55" s="25"/>
+      <c r="Q55" s="25"/>
       <c r="R55" s="11"/>
       <c r="S55" s="11"/>
       <c r="T55" s="11"/>
@@ -6556,7 +6592,7 @@
       <c r="BU55" s="11"/>
       <c r="BV55" s="12"/>
     </row>
-    <row r="56" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -6584,7 +6620,7 @@
       <c r="W56" s="11"/>
       <c r="X56" s="11"/>
       <c r="Y56" s="11"/>
-      <c r="Z56" s="24"/>
+      <c r="Z56" s="25"/>
       <c r="AA56"/>
       <c r="AB56" s="11"/>
       <c r="AC56" s="11"/>
@@ -6634,7 +6670,7 @@
       <c r="BU56" s="11"/>
       <c r="BV56" s="12"/>
     </row>
-    <row r="57" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -6651,7 +6687,7 @@
       <c r="L57" s="11"/>
       <c r="M57" s="11"/>
       <c r="N57" s="11"/>
-      <c r="O57" s="24"/>
+      <c r="O57" s="25"/>
       <c r="P57" s="11"/>
       <c r="Q57" s="11"/>
       <c r="R57" s="11"/>
@@ -6663,7 +6699,7 @@
       <c r="X57" s="11"/>
       <c r="Y57" s="11"/>
       <c r="Z57" s="11"/>
-      <c r="AA57" s="24"/>
+      <c r="AA57" s="25"/>
       <c r="AB57" s="11"/>
       <c r="AC57" s="11"/>
       <c r="AD57" s="11"/>
@@ -6712,7 +6748,7 @@
       <c r="BU57" s="11"/>
       <c r="BV57" s="12"/>
     </row>
-    <row r="58" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -6729,7 +6765,7 @@
       <c r="L58"/>
       <c r="M58" s="11"/>
       <c r="N58" s="11"/>
-      <c r="O58" s="24"/>
+      <c r="O58" s="25"/>
       <c r="P58" s="11"/>
       <c r="Q58" s="11"/>
       <c r="R58" s="11"/>
@@ -6741,7 +6777,7 @@
       <c r="X58" s="11"/>
       <c r="Y58" s="11"/>
       <c r="Z58" s="11"/>
-      <c r="AA58" s="24"/>
+      <c r="AA58" s="25"/>
       <c r="AB58" s="11"/>
       <c r="AC58" s="11"/>
       <c r="AD58" s="11"/>
@@ -6790,7 +6826,7 @@
       <c r="BU58" s="11"/>
       <c r="BV58" s="12"/>
     </row>
-    <row r="59" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -6803,7 +6839,7 @@
       <c r="H59" s="11"/>
       <c r="I59" s="11"/>
       <c r="J59" s="11"/>
-      <c r="K59" s="24"/>
+      <c r="K59" s="25"/>
       <c r="L59" s="11"/>
       <c r="M59" s="11"/>
       <c r="N59" s="11"/>
@@ -6819,7 +6855,7 @@
       <c r="X59" s="11"/>
       <c r="Y59" s="11"/>
       <c r="Z59" s="11"/>
-      <c r="AA59" s="24"/>
+      <c r="AA59" s="25"/>
       <c r="AB59" s="11"/>
       <c r="AC59" s="11"/>
       <c r="AD59" s="11"/>
@@ -6868,7 +6904,7 @@
       <c r="BU59" s="11"/>
       <c r="BV59" s="12"/>
     </row>
-    <row r="60" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -6881,11 +6917,11 @@
       <c r="H60" s="11"/>
       <c r="I60" s="11"/>
       <c r="J60" s="11"/>
-      <c r="K60" s="24"/>
+      <c r="K60" s="25"/>
       <c r="L60" s="11"/>
       <c r="M60" s="11"/>
       <c r="N60" s="11"/>
-      <c r="O60" s="24"/>
+      <c r="O60" s="25"/>
       <c r="P60" s="11"/>
       <c r="Q60" s="11"/>
       <c r="R60" s="11"/>
@@ -6897,7 +6933,7 @@
       <c r="X60" s="11"/>
       <c r="Y60" s="11"/>
       <c r="Z60" s="11"/>
-      <c r="AA60" s="24"/>
+      <c r="AA60" s="25"/>
       <c r="AB60" s="11"/>
       <c r="AC60" s="11"/>
       <c r="AD60" s="11"/>
@@ -6946,7 +6982,7 @@
       <c r="BU60" s="11"/>
       <c r="BV60" s="12"/>
     </row>
-    <row r="61" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -6960,13 +6996,13 @@
       <c r="I61" s="11"/>
       <c r="J61" s="11"/>
       <c r="K61" s="11"/>
-      <c r="L61" s="24"/>
+      <c r="L61" s="25"/>
       <c r="M61" s="11"/>
       <c r="N61" s="11"/>
       <c r="O61" s="11"/>
       <c r="P61" s="11"/>
       <c r="Q61" s="11"/>
-      <c r="R61" s="24"/>
+      <c r="R61" s="25"/>
       <c r="S61" s="11"/>
       <c r="T61"/>
       <c r="U61" s="11"/>
@@ -7024,7 +7060,7 @@
       <c r="BU61" s="11"/>
       <c r="BV61" s="12"/>
     </row>
-    <row r="62" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -7045,7 +7081,7 @@
       <c r="P62" s="11"/>
       <c r="Q62" s="11"/>
       <c r="R62"/>
-      <c r="S62" s="24"/>
+      <c r="S62" s="25"/>
       <c r="T62" s="11"/>
       <c r="U62" s="11"/>
       <c r="V62" s="11"/>
@@ -7102,7 +7138,7 @@
       <c r="BU62" s="11"/>
       <c r="BV62" s="12"/>
     </row>
-    <row r="63" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -7124,7 +7160,7 @@
       <c r="Q63" s="11"/>
       <c r="R63" s="11"/>
       <c r="S63"/>
-      <c r="T63" s="24"/>
+      <c r="T63" s="25"/>
       <c r="U63" s="11"/>
       <c r="V63" s="11"/>
       <c r="W63" s="11"/>
@@ -7180,7 +7216,7 @@
       <c r="BU63" s="11"/>
       <c r="BV63" s="12"/>
     </row>
-    <row r="64" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -7200,7 +7236,7 @@
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
       <c r="Q64" s="11"/>
-      <c r="R64" s="24"/>
+      <c r="R64" s="25"/>
       <c r="S64" s="11"/>
       <c r="T64"/>
       <c r="U64" s="11"/>
@@ -7258,7 +7294,7 @@
       <c r="BU64" s="11"/>
       <c r="BV64" s="12"/>
     </row>
-    <row r="65" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -7279,7 +7315,7 @@
       <c r="P65" s="11"/>
       <c r="Q65" s="11"/>
       <c r="R65" s="11"/>
-      <c r="S65" s="24"/>
+      <c r="S65" s="25"/>
       <c r="T65" s="11"/>
       <c r="U65" s="11"/>
       <c r="V65" s="11"/>
@@ -7336,7 +7372,7 @@
       <c r="BU65" s="11"/>
       <c r="BV65" s="12"/>
     </row>
-    <row r="66" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -7358,7 +7394,7 @@
       <c r="Q66" s="11"/>
       <c r="R66" s="11"/>
       <c r="S66" s="11"/>
-      <c r="T66" s="24"/>
+      <c r="T66" s="25"/>
       <c r="U66" s="11"/>
       <c r="V66" s="11"/>
       <c r="W66" s="11"/>
@@ -7414,7 +7450,7 @@
       <c r="BU66" s="11"/>
       <c r="BV66" s="12"/>
     </row>
-    <row r="67" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -7454,7 +7490,7 @@
       <c r="AI67" s="11"/>
       <c r="AJ67" s="11"/>
       <c r="AK67" s="11"/>
-      <c r="AL67" s="24"/>
+      <c r="AL67" s="25"/>
       <c r="AM67" s="11"/>
       <c r="AN67" s="11"/>
       <c r="AO67" s="11"/>
@@ -7492,7 +7528,7 @@
       <c r="BU67" s="11"/>
       <c r="BV67" s="12"/>
     </row>
-    <row r="68" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -7533,7 +7569,7 @@
       <c r="AJ68" s="11"/>
       <c r="AK68" s="11"/>
       <c r="AL68" s="11"/>
-      <c r="AM68" s="24"/>
+      <c r="AM68" s="25"/>
       <c r="AN68" s="11"/>
       <c r="AO68" s="11"/>
       <c r="AP68" s="11"/>
@@ -7570,7 +7606,7 @@
       <c r="BU68" s="11"/>
       <c r="BV68" s="12"/>
     </row>
-    <row r="69" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -7611,7 +7647,7 @@
       <c r="AJ69" s="11"/>
       <c r="AK69" s="11"/>
       <c r="AL69" s="11"/>
-      <c r="AM69" s="24"/>
+      <c r="AM69" s="25"/>
       <c r="AN69" s="11"/>
       <c r="AO69" s="11"/>
       <c r="AP69" s="11"/>
@@ -7648,7 +7684,7 @@
       <c r="BU69" s="11"/>
       <c r="BV69" s="12"/>
     </row>
-    <row r="70" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -7690,7 +7726,7 @@
       <c r="AK70" s="11"/>
       <c r="AL70" s="11"/>
       <c r="AM70" s="11"/>
-      <c r="AN70" s="24"/>
+      <c r="AN70" s="25"/>
       <c r="AO70" s="11"/>
       <c r="AP70" s="11"/>
       <c r="AQ70" s="11"/>
@@ -7726,7 +7762,7 @@
       <c r="BU70" s="11"/>
       <c r="BV70" s="12"/>
     </row>
-    <row r="71" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -7769,7 +7805,7 @@
       <c r="AL71" s="11"/>
       <c r="AM71" s="11"/>
       <c r="AN71" s="11"/>
-      <c r="AO71" s="24"/>
+      <c r="AO71" s="25"/>
       <c r="AP71" s="11"/>
       <c r="AQ71" s="11"/>
       <c r="AR71" s="11"/>
@@ -7804,7 +7840,7 @@
       <c r="BU71" s="11"/>
       <c r="BV71" s="12"/>
     </row>
-    <row r="72" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -7847,7 +7883,7 @@
       <c r="AL72" s="11"/>
       <c r="AM72" s="11"/>
       <c r="AN72" s="11"/>
-      <c r="AO72" s="24"/>
+      <c r="AO72" s="25"/>
       <c r="AP72" s="11"/>
       <c r="AQ72" s="11"/>
       <c r="AR72" s="11"/>
@@ -7882,7 +7918,7 @@
       <c r="BU72" s="11"/>
       <c r="BV72" s="12"/>
     </row>
-    <row r="73" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -7926,7 +7962,7 @@
       <c r="AM73" s="11"/>
       <c r="AN73" s="11"/>
       <c r="AO73" s="11"/>
-      <c r="AP73" s="24"/>
+      <c r="AP73" s="25"/>
       <c r="AQ73" s="11"/>
       <c r="AR73" s="11"/>
       <c r="AS73" s="11"/>
@@ -7960,7 +7996,7 @@
       <c r="BU73" s="11"/>
       <c r="BV73" s="12"/>
     </row>
-    <row r="74" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -8005,7 +8041,7 @@
       <c r="AN74" s="11"/>
       <c r="AO74" s="11"/>
       <c r="AP74" s="11"/>
-      <c r="AQ74" s="24"/>
+      <c r="AQ74" s="25"/>
       <c r="AR74" s="11"/>
       <c r="AS74" s="11"/>
       <c r="AT74" s="11"/>
@@ -8038,7 +8074,7 @@
       <c r="BU74" s="11"/>
       <c r="BV74" s="12"/>
     </row>
-    <row r="75" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -8084,7 +8120,7 @@
       <c r="AO75" s="11"/>
       <c r="AP75" s="11"/>
       <c r="AQ75" s="11"/>
-      <c r="AR75" s="24"/>
+      <c r="AR75" s="25"/>
       <c r="AS75" s="11"/>
       <c r="AT75" s="11"/>
       <c r="AU75" s="11"/>
@@ -8116,7 +8152,7 @@
       <c r="BU75" s="11"/>
       <c r="BV75" s="12"/>
     </row>
-    <row r="76" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -8163,7 +8199,7 @@
       <c r="AP76" s="11"/>
       <c r="AQ76" s="11"/>
       <c r="AR76" s="11"/>
-      <c r="AS76" s="24"/>
+      <c r="AS76" s="25"/>
       <c r="AT76" s="11"/>
       <c r="AU76" s="11"/>
       <c r="AV76" s="11"/>
@@ -8194,7 +8230,7 @@
       <c r="BU76" s="11"/>
       <c r="BV76" s="12"/>
     </row>
-    <row r="77" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -8242,7 +8278,7 @@
       <c r="AQ77" s="11"/>
       <c r="AR77" s="11"/>
       <c r="AS77" s="11"/>
-      <c r="AT77" s="24"/>
+      <c r="AT77" s="25"/>
       <c r="AU77" s="11"/>
       <c r="AV77" s="11"/>
       <c r="AW77" s="11"/>
@@ -8272,7 +8308,7 @@
       <c r="BU77" s="11"/>
       <c r="BV77" s="12"/>
     </row>
-    <row r="78" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -8321,7 +8357,7 @@
       <c r="AR78" s="11"/>
       <c r="AS78" s="11"/>
       <c r="AT78" s="11"/>
-      <c r="AU78" s="24"/>
+      <c r="AU78" s="25"/>
       <c r="AV78" s="11"/>
       <c r="AW78" s="11"/>
       <c r="AX78" s="11"/>
@@ -8350,7 +8386,7 @@
       <c r="BU78" s="11"/>
       <c r="BV78" s="12"/>
     </row>
-    <row r="79" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -8400,7 +8436,7 @@
       <c r="AS79" s="11"/>
       <c r="AT79" s="11"/>
       <c r="AU79" s="11"/>
-      <c r="AV79" s="24"/>
+      <c r="AV79" s="25"/>
       <c r="AW79" s="11"/>
       <c r="AX79" s="11"/>
       <c r="AY79" s="11"/>
@@ -8428,7 +8464,7 @@
       <c r="BU79" s="11"/>
       <c r="BV79" s="12"/>
     </row>
-    <row r="80" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -8479,7 +8515,7 @@
       <c r="AT80" s="11"/>
       <c r="AU80" s="11"/>
       <c r="AV80" s="11"/>
-      <c r="AW80" s="24"/>
+      <c r="AW80" s="25"/>
       <c r="AX80" s="11"/>
       <c r="AY80" s="11"/>
       <c r="AZ80" s="11"/>
@@ -8506,7 +8542,7 @@
       <c r="BU80" s="11"/>
       <c r="BV80" s="12"/>
     </row>
-    <row r="81" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -8558,7 +8594,7 @@
       <c r="AU81" s="11"/>
       <c r="AV81" s="11"/>
       <c r="AW81" s="11"/>
-      <c r="AX81" s="24"/>
+      <c r="AX81" s="25"/>
       <c r="AY81" s="11"/>
       <c r="AZ81" s="11"/>
       <c r="BA81" s="11"/>
@@ -8584,7 +8620,7 @@
       <c r="BU81" s="11"/>
       <c r="BV81" s="12"/>
     </row>
-    <row r="82" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -8637,7 +8673,7 @@
       <c r="AV82" s="11"/>
       <c r="AW82" s="11"/>
       <c r="AX82" s="11"/>
-      <c r="AY82" s="24"/>
+      <c r="AY82" s="25"/>
       <c r="AZ82" s="11"/>
       <c r="BA82" s="11"/>
       <c r="BB82" s="11"/>
@@ -8662,7 +8698,7 @@
       <c r="BU82" s="11"/>
       <c r="BV82" s="12"/>
     </row>
-    <row r="83" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -8716,7 +8752,7 @@
       <c r="AW83" s="11"/>
       <c r="AX83" s="11"/>
       <c r="AY83" s="11"/>
-      <c r="AZ83" s="24"/>
+      <c r="AZ83" s="25"/>
       <c r="BA83" s="11"/>
       <c r="BB83" s="11"/>
       <c r="BC83" s="11"/>
@@ -8740,7 +8776,7 @@
       <c r="BU83" s="11"/>
       <c r="BV83" s="12"/>
     </row>
-    <row r="84" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -8795,7 +8831,7 @@
       <c r="AX84" s="11"/>
       <c r="AY84" s="11"/>
       <c r="AZ84" s="11"/>
-      <c r="BA84" s="24"/>
+      <c r="BA84" s="25"/>
       <c r="BB84" s="11"/>
       <c r="BC84" s="11"/>
       <c r="BD84" s="11"/>
@@ -8818,7 +8854,7 @@
       <c r="BU84" s="11"/>
       <c r="BV84" s="12"/>
     </row>
-    <row r="85" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -8874,7 +8910,7 @@
       <c r="AY85" s="11"/>
       <c r="AZ85" s="11"/>
       <c r="BA85" s="11"/>
-      <c r="BB85" s="24"/>
+      <c r="BB85" s="25"/>
       <c r="BC85" s="11"/>
       <c r="BD85" s="11"/>
       <c r="BE85" s="11"/>
@@ -8896,7 +8932,7 @@
       <c r="BU85" s="11"/>
       <c r="BV85" s="12"/>
     </row>
-    <row r="86" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -8953,7 +8989,7 @@
       <c r="AZ86" s="11"/>
       <c r="BA86" s="11"/>
       <c r="BB86" s="11"/>
-      <c r="BC86" s="24"/>
+      <c r="BC86" s="25"/>
       <c r="BD86" s="11"/>
       <c r="BE86" s="11"/>
       <c r="BF86" s="11"/>
@@ -8974,7 +9010,7 @@
       <c r="BU86" s="11"/>
       <c r="BV86" s="12"/>
     </row>
-    <row r="87" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -9032,7 +9068,7 @@
       <c r="BA87" s="11"/>
       <c r="BB87" s="11"/>
       <c r="BC87" s="11"/>
-      <c r="BD87" s="24"/>
+      <c r="BD87" s="25"/>
       <c r="BE87" s="11"/>
       <c r="BF87" s="11"/>
       <c r="BG87" s="11"/>
@@ -9052,7 +9088,7 @@
       <c r="BU87" s="11"/>
       <c r="BV87" s="12"/>
     </row>
-    <row r="88" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -9111,7 +9147,7 @@
       <c r="BB88" s="11"/>
       <c r="BC88" s="11"/>
       <c r="BD88" s="11"/>
-      <c r="BE88" s="24"/>
+      <c r="BE88" s="25"/>
       <c r="BF88" s="11"/>
       <c r="BG88" s="11"/>
       <c r="BH88" s="11"/>
@@ -9130,7 +9166,7 @@
       <c r="BU88" s="11"/>
       <c r="BV88" s="12"/>
     </row>
-    <row r="89" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -9190,7 +9226,7 @@
       <c r="BC89" s="11"/>
       <c r="BD89" s="11"/>
       <c r="BE89" s="11"/>
-      <c r="BF89" s="24"/>
+      <c r="BF89" s="25"/>
       <c r="BG89" s="11"/>
       <c r="BH89" s="11"/>
       <c r="BI89" s="11"/>
@@ -9208,7 +9244,7 @@
       <c r="BU89" s="11"/>
       <c r="BV89" s="12"/>
     </row>
-    <row r="90" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -9269,7 +9305,7 @@
       <c r="BD90" s="11"/>
       <c r="BE90" s="11"/>
       <c r="BF90" s="11"/>
-      <c r="BG90" s="24"/>
+      <c r="BG90" s="25"/>
       <c r="BH90" s="11"/>
       <c r="BI90" s="11"/>
       <c r="BJ90" s="11"/>
@@ -9286,7 +9322,7 @@
       <c r="BU90" s="11"/>
       <c r="BV90" s="12"/>
     </row>
-    <row r="91" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -9348,7 +9384,7 @@
       <c r="BE91" s="11"/>
       <c r="BF91" s="11"/>
       <c r="BG91" s="11"/>
-      <c r="BH91" s="24"/>
+      <c r="BH91" s="25"/>
       <c r="BI91" s="11"/>
       <c r="BJ91" s="11"/>
       <c r="BK91" s="11"/>
@@ -9364,7 +9400,7 @@
       <c r="BU91" s="11"/>
       <c r="BV91" s="12"/>
     </row>
-    <row r="92" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -9427,7 +9463,7 @@
       <c r="BF92" s="11"/>
       <c r="BG92" s="11"/>
       <c r="BH92" s="11"/>
-      <c r="BI92" s="24"/>
+      <c r="BI92" s="25"/>
       <c r="BJ92" s="11"/>
       <c r="BK92" s="11"/>
       <c r="BL92" s="11"/>
@@ -9442,7 +9478,7 @@
       <c r="BU92" s="11"/>
       <c r="BV92" s="12"/>
     </row>
-    <row r="93" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -9506,7 +9542,7 @@
       <c r="BG93" s="11"/>
       <c r="BH93" s="11"/>
       <c r="BI93" s="11"/>
-      <c r="BJ93" s="24"/>
+      <c r="BJ93" s="25"/>
       <c r="BK93" s="11"/>
       <c r="BL93" s="11"/>
       <c r="BM93" s="11"/>
@@ -9520,7 +9556,7 @@
       <c r="BU93" s="11"/>
       <c r="BV93" s="12"/>
     </row>
-    <row r="94" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -9585,7 +9621,7 @@
       <c r="BH94" s="11"/>
       <c r="BI94" s="11"/>
       <c r="BJ94" s="11"/>
-      <c r="BK94" s="24"/>
+      <c r="BK94" s="25"/>
       <c r="BL94" s="11"/>
       <c r="BM94" s="11"/>
       <c r="BN94" s="11"/>
@@ -9598,7 +9634,7 @@
       <c r="BU94" s="11"/>
       <c r="BV94" s="12"/>
     </row>
-    <row r="95" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -9664,7 +9700,7 @@
       <c r="BI95" s="11"/>
       <c r="BJ95" s="11"/>
       <c r="BK95" s="11"/>
-      <c r="BL95" s="24"/>
+      <c r="BL95" s="25"/>
       <c r="BM95" s="11"/>
       <c r="BN95" s="11"/>
       <c r="BO95" s="11"/>
@@ -9676,7 +9712,7 @@
       <c r="BU95" s="11"/>
       <c r="BV95" s="12"/>
     </row>
-    <row r="96" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -9743,7 +9779,7 @@
       <c r="BJ96" s="11"/>
       <c r="BK96" s="11"/>
       <c r="BL96" s="11"/>
-      <c r="BM96" s="24"/>
+      <c r="BM96" s="25"/>
       <c r="BN96" s="11"/>
       <c r="BO96" s="11"/>
       <c r="BP96" s="11"/>
@@ -9754,7 +9790,7 @@
       <c r="BU96" s="11"/>
       <c r="BV96" s="12"/>
     </row>
-    <row r="97" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -9822,7 +9858,7 @@
       <c r="BK97" s="11"/>
       <c r="BL97" s="11"/>
       <c r="BM97" s="11"/>
-      <c r="BN97" s="24"/>
+      <c r="BN97" s="25"/>
       <c r="BO97" s="11"/>
       <c r="BP97" s="11"/>
       <c r="BQ97" s="11"/>
@@ -9832,7 +9868,7 @@
       <c r="BU97" s="11"/>
       <c r="BV97" s="12"/>
     </row>
-    <row r="98" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -9901,7 +9937,7 @@
       <c r="BL98" s="11"/>
       <c r="BM98" s="11"/>
       <c r="BN98" s="11"/>
-      <c r="BO98" s="24"/>
+      <c r="BO98" s="25"/>
       <c r="BP98" s="11"/>
       <c r="BQ98" s="11"/>
       <c r="BR98" s="11"/>
@@ -9910,7 +9946,7 @@
       <c r="BU98" s="11"/>
       <c r="BV98" s="12"/>
     </row>
-    <row r="99" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -9980,7 +10016,7 @@
       <c r="BM99" s="11"/>
       <c r="BN99" s="11"/>
       <c r="BO99" s="11"/>
-      <c r="BP99" s="24"/>
+      <c r="BP99" s="25"/>
       <c r="BQ99" s="11"/>
       <c r="BR99" s="11"/>
       <c r="BS99" s="11"/>
@@ -9988,7 +10024,7 @@
       <c r="BU99" s="11"/>
       <c r="BV99" s="12"/>
     </row>
-    <row r="100" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -10059,14 +10095,14 @@
       <c r="BN100" s="11"/>
       <c r="BO100" s="11"/>
       <c r="BP100" s="11"/>
-      <c r="BQ100" s="24"/>
+      <c r="BQ100" s="25"/>
       <c r="BR100" s="11"/>
       <c r="BS100" s="11"/>
       <c r="BT100" s="11"/>
       <c r="BU100" s="11"/>
       <c r="BV100" s="12"/>
     </row>
-    <row r="101" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -10138,13 +10174,13 @@
       <c r="BO101" s="11"/>
       <c r="BP101" s="11"/>
       <c r="BQ101" s="11"/>
-      <c r="BR101" s="24"/>
+      <c r="BR101" s="25"/>
       <c r="BS101" s="11"/>
       <c r="BT101" s="11"/>
       <c r="BU101" s="11"/>
       <c r="BV101" s="12"/>
     </row>
-    <row r="102" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -10217,12 +10253,12 @@
       <c r="BP102" s="11"/>
       <c r="BQ102" s="11"/>
       <c r="BR102" s="11"/>
-      <c r="BS102" s="24"/>
+      <c r="BS102" s="25"/>
       <c r="BT102" s="11"/>
       <c r="BU102" s="11"/>
       <c r="BV102" s="12"/>
     </row>
-    <row r="103" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
         <v>102</v>
       </c>
@@ -10296,11 +10332,11 @@
       <c r="BQ103" s="11"/>
       <c r="BR103" s="11"/>
       <c r="BS103" s="11"/>
-      <c r="BT103" s="24"/>
+      <c r="BT103" s="25"/>
       <c r="BU103" s="11"/>
       <c r="BV103" s="12"/>
     </row>
-    <row r="104" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
         <v>103</v>
       </c>
@@ -10375,10 +10411,10 @@
       <c r="BR104" s="11"/>
       <c r="BS104" s="11"/>
       <c r="BT104" s="11"/>
-      <c r="BU104" s="24"/>
+      <c r="BU104" s="25"/>
       <c r="BV104" s="12"/>
     </row>
-    <row r="105" spans="1:74" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:74" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
         <v>104</v>
       </c>
@@ -10454,9 +10490,9 @@
       <c r="BS105" s="14"/>
       <c r="BT105" s="14"/>
       <c r="BU105" s="14"/>
-      <c r="BV105" s="24"/>
-    </row>
-    <row r="106" spans="1:74" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="BV105" s="28"/>
+    </row>
+    <row r="106" spans="1:74" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>